<commit_message>
added new classes and updated existing classes
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/devicecontrol/testdata/ProfilesThemesData.xlsx
+++ b/src/main/java/com/qa/devicecontrol/testdata/ProfilesThemesData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vasu\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D57F294-0FA3-4C2D-9A5F-67443077D66E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333A933E-2F84-4154-9463-733E4599CC32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RoomDisplayProfileData" sheetId="1" r:id="rId1"/>
+    <sheet name="RoomDisplayData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>ProfileName</t>
+    <t>Test RoomDisplay EventsView</t>
   </si>
   <si>
-    <t>Test RoomDisplay EventsView</t>
+    <t>EventsProfileName</t>
   </si>
 </sst>
 </file>
@@ -376,12 +376,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>